<commit_message>
change top k in reranker
</commit_message>
<xml_diff>
--- a/evaluate/data/data_evaluate_DaNang.xlsx
+++ b/evaluate/data/data_evaluate_DaNang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TDTU\Year_4_Semester1\Dự án\Code\evaluate\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F22352E-76CA-4E08-93A8-61B3560FA853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B7C58A-CE5E-4AB2-8C71-E7392B1A4601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1027,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1279,7 +1279,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>60</v>
       </c>
@@ -1287,567 +1287,563 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B102" s="3" t="s">
         <v>201</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Evaluate for rag at TPHCM and Da Nang
</commit_message>
<xml_diff>
--- a/evaluate/data/data_evaluate_DaNang.xlsx
+++ b/evaluate/data/data_evaluate_DaNang.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TDTU\Year_4_Semester1\Dự án\Code\evaluate\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DBF347-76B5-441F-B5E3-E39C7B8D6D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517FA5D5-936A-4944-9A76-BE85991572FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -177,12 +186,6 @@
     <t>Nổi bật có tàu lượn siêu tốc Queen Cobra, tháp rơi tự do, Singapore Sling, Ninja Flyer, Festival Carousel, Dino Island, và Sky Treasure – những trò chơi cảm giác mạnh và giải trí cho cả gia đình.</t>
   </si>
   <si>
-    <t>Món ăn nào ở Đà Nẵng được xem là đặc sản đêm khiến du khách nhớ mãi?</t>
-  </si>
-  <si>
-    <t>Các món ăn đêm được yêu thích gồm bánh mì Ông Tý, bánh canh Bà Bé, cháo trắng hột vịt muối 100, bánh xèo Bà Dưỡng và cơm thố tiệm Chợ Lớn – đều mang đậm hương vị đặc trưng Đà Nẵng.</t>
-  </si>
-  <si>
     <t>Tiệm ăn Chợ Lớn ở Đà Nẵng nổi tiếng với món gì và phục vụ đến mấy giờ?</t>
   </si>
   <si>
@@ -615,9 +618,6 @@
     <t>Gồm chả bò Đà Nẵng, bánh khô mè, mực rim me, rong biển Mỹ Khê, nước mắm Nam Ô, mực một nắng. Mua tại cơ sở Lê Trọng Thịnh, Bà Hường, Bà Liễu Mẹ, Cẩm Lệ.</t>
   </si>
   <si>
-    <t>ường nào tại Đà Nẵng được xem là “thiên đường ẩm thực” về đêm?</t>
-  </si>
-  <si>
     <t>Đường Phạm Hồng Thái, nơi tập trung cơm gà, mì xíu khô, bún bò và các món ăn vặt đậm chất địa phương, là “thiên đường” ẩm thực đêm của Đà Nẵng.</t>
   </si>
   <si>
@@ -631,6 +631,15 @@
   </si>
   <si>
     <t>Món mì vàng dai nhẹ, ăn với thịt heo xá xíu, rau sống, nước dùng đặc trưng, gắn liền với thương cảng Hội An – Đà Nẵng. Địa chỉ: Cao Lầu Hoài Phố (255 Nguyễn Chí Thanh), Cao Lầu Phố Hội (163 Phan Đăng Lưu).</t>
+  </si>
+  <si>
+    <t>Đường nào tại Đà Nẵng được xem là “thiên đường ẩm thực” về đêm?</t>
+  </si>
+  <si>
+    <t>43 Factory Coffee Roaster có phong cách như thế nào và phục vụ gì?</t>
+  </si>
+  <si>
+    <t>Quán có không gian công nghiệp hiện đại, quầy bar 360 độ và đầy đủ dụng cụ pha chế chuyên nghiệp. Chuyên phục vụ cà phê arabica chất lượng cao với menu đa dạng như espresso, cold brew, cà phê sữa đá và món tráng miệng. Là quán yêu thích của giới sành cà phê, địa chỉ 422 Ngô Thì Sỹ.</t>
   </si>
 </sst>
 </file>
@@ -659,7 +668,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -669,6 +678,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF535FC1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -745,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -757,6 +772,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1041,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90:B91"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90:B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,10 +1206,10 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1435,7 +1453,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>96</v>
       </c>
@@ -1443,7 +1461,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>98</v>
       </c>
@@ -1451,7 +1469,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>100</v>
       </c>
@@ -1459,7 +1477,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>102</v>
       </c>
@@ -1467,7 +1485,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>104</v>
       </c>
@@ -1475,7 +1493,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>106</v>
       </c>
@@ -1491,7 +1509,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>110</v>
       </c>
@@ -1499,7 +1517,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>112</v>
       </c>
@@ -1555,7 +1573,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>126</v>
       </c>
@@ -1571,7 +1589,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>130</v>
       </c>
@@ -1579,7 +1597,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>132</v>
       </c>
@@ -1587,7 +1605,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>134</v>
       </c>
@@ -1611,7 +1629,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>140</v>
       </c>
@@ -1635,7 +1653,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>146</v>
       </c>
@@ -1691,7 +1709,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>160</v>
       </c>
@@ -1699,7 +1717,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>162</v>
       </c>
@@ -1739,47 +1757,47 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B88" s="4" t="s">
+      <c r="A88" s="5" t="s">
         <v>195</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B89" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="5" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="4" t="s">
+      <c r="B90" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="B90" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>174</v>
       </c>
@@ -1787,7 +1805,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
         <v>176</v>
       </c>
@@ -1803,7 +1821,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>180</v>
       </c>
@@ -1851,12 +1869,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>